<commit_message>
Avance: Implementación del módulo Programa Anual y mejoras en el sistema avanze 2
</commit_message>
<xml_diff>
--- a/recursos-panel/reports/base/xlsx base reporte.xlsx
+++ b/recursos-panel/reports/base/xlsx base reporte.xlsx
@@ -1,107 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\sistemaInventario\recursos-panel\reports\base\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp1\htdocs\sistema_inventario\recursos-panel\reports\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD197ABB-4408-4A7B-98DE-593C0CE2DCD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C6C62E-E3F5-450B-B860-F5EAEC0694F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Formato" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="179021"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t xml:space="preserve">Nombre del Laboratorio: </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">
-Subproceso de apoyo: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Laboratorios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Formato: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>Existencia de materiales, equipos e insumos de laboratorios</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-Fecha de aprobación: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>06 de enero de 2022</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-  </si>
-  <si>
-    <t>OPEN SOURCE</t>
   </si>
   <si>
     <t xml:space="preserve">No. </t>
   </si>
   <si>
-    <t xml:space="preserve">
-Nombre del equipo, material e insumos</t>
-  </si>
-  <si>
-    <t>Cantidad</t>
-  </si>
-  <si>
     <t>Unidad</t>
-  </si>
-  <si>
-    <t>Código interno</t>
   </si>
   <si>
     <t>Marca</t>
@@ -113,17 +40,75 @@
     <t>Observaciones</t>
   </si>
   <si>
-    <t>En servicio</t>
+    <t>Descripcion del producto</t>
   </si>
   <si>
-    <t>Fuera de servicio</t>
+    <t>Codigo Interno</t>
+  </si>
+  <si>
+    <t>Proveedor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Subproceso de Apoyo: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Laboratorios </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Formato: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Existencia de Materiales e Insumos de Laboratorios
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Fecha de aprobación: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>octubre 2023</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -166,24 +151,21 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -200,7 +182,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -307,49 +289,34 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -360,7 +327,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -382,104 +349,83 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -569,34 +515,34 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>275872</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>58561</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>352425</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>801511</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
+      <xdr:rowOff>115711</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1312" name="2 Imagen" descr="UPT02">
+        <xdr:cNvPr id="4" name="image1.jpg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000020050000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1337FD1D-430A-486B-A3EE-C852D4AF0797}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -610,16 +556,13 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="495300" y="66675"/>
-          <a:ext cx="1028700" cy="704850"/>
+          <a:off x="7349772" y="58561"/>
+          <a:ext cx="1605139" cy="685800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
         <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
             <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
@@ -628,40 +571,30 @@
               </a:solidFill>
             </a14:hiddenFill>
           </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
-    <xdr:clientData/>
+    <xdr:clientData fLocksWithSheet="0"/>
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>209550</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>42333</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>155222</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>815065</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>28222</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1313" name="Imagen 1">
+        <xdr:cNvPr id="3" name="Imagen 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000021050000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D503DAEF-6D4A-4BD1-881D-0482A041AD47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -670,49 +603,25 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="7829550" y="104775"/>
-          <a:ext cx="1171575" cy="561975"/>
+          <a:off x="282222" y="155222"/>
+          <a:ext cx="1788732" cy="508000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-              <a:solidFill>
-                <a:srgbClr val="FFFFFF"/>
-              </a:solidFill>
-            </a14:hiddenFill>
-          </a:ext>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1044,86 +953,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:M237"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:M9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.42578125" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="4" max="4" width="4.85546875" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" customWidth="1"/>
-    <col min="6" max="6" width="8.140625" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" customWidth="1"/>
-    <col min="8" max="8" width="25.42578125" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" customWidth="1"/>
-    <col min="12" max="12" width="12.7109375" customWidth="1"/>
-    <col min="13" max="13" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" width="4.6328125" customWidth="1"/>
+    <col min="2" max="2" width="4.26953125" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="4" max="4" width="12.1796875" customWidth="1"/>
+    <col min="5" max="5" width="7.54296875" customWidth="1"/>
+    <col min="6" max="6" width="8.1796875" customWidth="1"/>
+    <col min="7" max="7" width="9.54296875" customWidth="1"/>
+    <col min="8" max="8" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" customWidth="1"/>
+    <col min="10" max="10" width="21.81640625" customWidth="1"/>
+    <col min="11" max="11" width="15.453125" customWidth="1"/>
+    <col min="12" max="12" width="12.7265625" customWidth="1"/>
+    <col min="13" max="13" width="10.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="11" t="s">
-        <v>1</v>
+    <row r="1" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="13"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="26" t="s">
+        <v>9</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="12"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="28"/>
     </row>
-    <row r="2" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="23"/>
+    <row r="2" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="13"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="30"/>
+      <c r="G2" s="30"/>
+      <c r="H2" s="30"/>
+      <c r="I2" s="30"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="31"/>
     </row>
-    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="27"/>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
-      <c r="K3" s="16"/>
-      <c r="L3" s="22"/>
-      <c r="M3" s="23"/>
+    <row r="3" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="13"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="30"/>
+      <c r="K3" s="29"/>
+      <c r="L3" s="31"/>
     </row>
-    <row r="4" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="25"/>
+    <row r="4" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="16"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="34"/>
     </row>
-    <row r="5" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -1137,84 +1042,77 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
     </row>
-    <row r="6" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="26"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="10" t="s">
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19"/>
+      <c r="I6" s="19"/>
+      <c r="J6" s="19"/>
+      <c r="K6" s="19"/>
+      <c r="L6" s="19"/>
+    </row>
+    <row r="8" spans="2:13" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C8" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="8" spans="2:13" s="4" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
+      <c r="G8" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="I8" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="30"/>
-      <c r="E8" s="31"/>
-      <c r="F8" s="28" t="s">
+      <c r="K8" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="28" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="32" t="s">
-        <v>7</v>
-      </c>
-      <c r="I8" s="28" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="K8" s="34"/>
-      <c r="L8" s="35" t="s">
-        <v>10</v>
-      </c>
-      <c r="M8" s="31"/>
+      <c r="L8" s="11"/>
+      <c r="M8"/>
     </row>
-    <row r="9" spans="2:13" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="36"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="38"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="40"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="L9" s="37"/>
-      <c r="M9" s="39"/>
+    <row r="9" spans="2:13" s="4" customFormat="1" ht="12.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
     </row>
-    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="208" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B227" s="7"/>
       <c r="C227" s="7"/>
       <c r="D227" s="7"/>
@@ -1228,7 +1126,7 @@
       <c r="L227" s="7"/>
       <c r="M227" s="7"/>
     </row>
-    <row r="228" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="228" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B228" s="7"/>
       <c r="C228" s="7"/>
       <c r="D228" s="7"/>
@@ -1242,7 +1140,7 @@
       <c r="L228" s="7"/>
       <c r="M228" s="7"/>
     </row>
-    <row r="231" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="231" spans="2:13" ht="13" x14ac:dyDescent="0.3">
       <c r="C231" s="1"/>
       <c r="D231" s="1"/>
       <c r="E231" s="1"/>
@@ -1255,26 +1153,20 @@
       <c r="L231" s="1"/>
       <c r="M231" s="1"/>
     </row>
-    <row r="237" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="237" spans="2:13" ht="13" x14ac:dyDescent="0.3">
       <c r="G237" s="1"/>
       <c r="H237" s="1"/>
       <c r="K237" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L8:M9"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="C8:E9"/>
-    <mergeCell ref="F8:F9"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
+  <mergeCells count="7">
     <mergeCell ref="F6:L6"/>
-    <mergeCell ref="E1:K4"/>
-    <mergeCell ref="L1:M4"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="B1:D4"/>
+    <mergeCell ref="E1:J4"/>
+    <mergeCell ref="K1:L4"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="K8:L8"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.51181102362204722" right="0.59055118110236227" top="0.43307086614173229" bottom="0.35433070866141736" header="0" footer="0"/>

</xml_diff>

<commit_message>
Actualización: Mejoras en módulo de Perfil y ajustes generales fase 3
</commit_message>
<xml_diff>
--- a/recursos-panel/reports/base/xlsx base reporte.xlsx
+++ b/recursos-panel/reports/base/xlsx base reporte.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp1\htdocs\sistema_inventario\recursos-panel\reports\base\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C6C62E-E3F5-450B-B860-F5EAEC0694F7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C60D8047-91D8-412C-A948-DEDA5CE7B526}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -616,8 +616,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="282222" y="155222"/>
-          <a:ext cx="1788732" cy="508000"/>
+          <a:off x="366183" y="155222"/>
+          <a:ext cx="1788732" cy="501650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -954,7 +954,7 @@
   <dimension ref="B1:M237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E1" sqref="E1:J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>

</xml_diff>